<commit_message>
last commit for assignment 1
</commit_message>
<xml_diff>
--- a/Assignment1-guess-number/Iteration5/document/defect_log.xlsx
+++ b/Assignment1-guess-number/Iteration5/document/defect_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shukebeta/OneDrive - Ara Institute of Canterbury/BCPR280/Assignment1-guess-number/Iteration3/document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shukebeta/OneDrive - Ara Institute of Canterbury/BCPR280/Assignment1-guess-number/Iteration5/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{8B0F8C2A-4FB5-4340-A86C-82FC343803F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{CEB43886-4DFF-3941-9C77-12B24CEF41B8}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{8B0F8C2A-4FB5-4340-A86C-82FC343803F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{844E7C8F-95D2-DE4B-8F76-82D7FF62038F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,37 +622,37 @@
     <t>2min</t>
   </si>
   <si>
-    <t>adjust requirement: more than 40 adjust to "more than 40 or equal to 40"</t>
-  </si>
-  <si>
     <t>Amitrajit Sarkar</t>
   </si>
   <si>
-    <t>Forgot handle "correct" branch: set Start button text and output computer win message.</t>
-  </si>
-  <si>
-    <t>add this. to currentGame</t>
-  </si>
-  <si>
-    <t>Forgot add this. prefix to data variable: currentGame</t>
-  </si>
-  <si>
-    <t>complain message with wrong information: I should use guess attribute but used result</t>
-  </si>
-  <si>
-    <t>change the attribute name</t>
-  </si>
-  <si>
-    <t>when computer guess 2, the guess message will disappear</t>
-  </si>
-  <si>
-    <t>modify the v-if condition</t>
-  </si>
-  <si>
-    <t>When computer find mankind lying, the game should end but it didn't</t>
-  </si>
-  <si>
-    <t>end the game</t>
+    <t>The guess history display too large</t>
+  </si>
+  <si>
+    <t>refine the list item sytle</t>
+  </si>
+  <si>
+    <t>The Start button is too small</t>
+  </si>
+  <si>
+    <t>refine the Start button style</t>
+  </si>
+  <si>
+    <t>The feedback button isn't align good</t>
+  </si>
+  <si>
+    <t>adjust the feedback button align</t>
+  </si>
+  <si>
+    <t>extend the padding</t>
+  </si>
+  <si>
+    <t>The padding under the header  is too narrow</t>
+  </si>
+  <si>
+    <t>The margin of the application is not good</t>
+  </si>
+  <si>
+    <t>refine the margin</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1353,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1382,9 +1382,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="32">
+    <row r="7" spans="1:8" ht="16">
       <c r="A7" s="18">
-        <v>43561</v>
+        <v>43575</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1402,15 +1402,15 @@
         <v>68</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16">
       <c r="A8" s="18">
-        <v>43555</v>
+        <v>43575</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1428,15 +1428,15 @@
         <v>69</v>
       </c>
       <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
       <c r="A9" s="18">
-        <v>43555</v>
+        <v>43575</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="10" spans="1:8" ht="16">
       <c r="A10" s="18">
-        <v>43555</v>
+        <v>43575</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1480,15 +1480,15 @@
         <v>72</v>
       </c>
       <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16">
       <c r="A11" s="18">
-        <v>43555</v>
+        <v>43575</v>
       </c>
       <c r="B11">
         <v>5</v>

</xml_diff>